<commit_message>
added new antibody HC84.27 and binding location 446
</commit_message>
<xml_diff>
--- a/tabular/antibodyEpitopeTable.xlsx
+++ b/tabular/antibodyEpitopeTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="460" windowWidth="34580" windowHeight="16240" activeTab="2"/>
+    <workbookView xWindow="15440" yWindow="1400" windowWidth="34580" windowHeight="22740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="246">
   <si>
     <t xml:space="preserve">Epitope </t>
   </si>
@@ -3656,13 +3656,52 @@
   </si>
   <si>
     <t>BR9</t>
+  </si>
+  <si>
+    <t>HC84.27</t>
+  </si>
+  <si>
+    <t>K446</t>
+  </si>
+  <si>
+    <r>
+      <t>NTGWLAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YQH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>K</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3697,6 +3736,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5142,10 +5186,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:V58"/>
+  <dimension ref="B1:V59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6104,54 +6148,57 @@
         <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>243</v>
       </c>
       <c r="D42" t="s">
         <v>47</v>
       </c>
       <c r="E42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" t="s">
+        <v>244</v>
+      </c>
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
+      <c r="O42" t="s">
+        <v>245</v>
+      </c>
+      <c r="R42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
         <v>73</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>133</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>27</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H43" t="s">
         <v>82</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O43" t="s">
         <v>134</v>
       </c>
-      <c r="R42" t="s">
+      <c r="R43" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G44" t="s">
-        <v>27</v>
-      </c>
-      <c r="H44" t="s">
-        <v>82</v>
-      </c>
-      <c r="O44" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
@@ -6159,7 +6206,7 @@
         <v>122</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>48</v>
@@ -6173,8 +6220,11 @@
       <c r="G45" t="s">
         <v>27</v>
       </c>
+      <c r="H45" t="s">
+        <v>82</v>
+      </c>
       <c r="O45" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
@@ -6182,25 +6232,22 @@
         <v>122</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H46" t="s">
         <v>27</v>
       </c>
       <c r="O46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
@@ -6208,22 +6255,25 @@
         <v>122</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s">
         <v>25</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>26</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>27</v>
       </c>
       <c r="O47" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
@@ -6231,7 +6281,7 @@
         <v>122</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>48</v>
@@ -6245,11 +6295,8 @@
       <c r="G48" t="s">
         <v>27</v>
       </c>
-      <c r="H48" t="s">
-        <v>82</v>
-      </c>
       <c r="O48" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.2">
@@ -6257,59 +6304,53 @@
         <v>122</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" t="s">
+        <v>82</v>
       </c>
       <c r="O49" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" t="s">
-        <v>47</v>
+      <c r="C50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E50" t="s">
         <v>80</v>
       </c>
       <c r="F50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50" t="s">
-        <v>25</v>
-      </c>
-      <c r="H50" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" t="s">
-        <v>27</v>
-      </c>
-      <c r="J50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O50" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>122</v>
       </c>
-      <c r="C51" t="s">
-        <v>138</v>
+      <c r="C51" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -6341,22 +6382,31 @@
         <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
       </c>
       <c r="E52" t="s">
+        <v>80</v>
+      </c>
+      <c r="F52" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H52" t="s">
         <v>26</v>
       </c>
-      <c r="F52" t="s">
+      <c r="I52" t="s">
         <v>27</v>
       </c>
-      <c r="G52" t="s">
-        <v>140</v>
+      <c r="J52" t="s">
+        <v>82</v>
       </c>
       <c r="O52" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.2">
@@ -6364,92 +6414,74 @@
         <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
       </c>
       <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" t="s">
+        <v>140</v>
+      </c>
+      <c r="O53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" t="s">
         <v>142</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>26</v>
       </c>
-      <c r="O53" t="s">
+      <c r="O54" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>145</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>144</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>47</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>80</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
         <v>81</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>63</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>64</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I56" t="s">
         <v>104</v>
       </c>
-      <c r="O55" t="s">
+      <c r="O56" t="s">
         <v>146</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S56" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" t="s">
-        <v>164</v>
-      </c>
-      <c r="D57" t="s">
-        <v>47</v>
-      </c>
-      <c r="E57" t="s">
-        <v>166</v>
-      </c>
-      <c r="F57" t="s">
-        <v>167</v>
-      </c>
-      <c r="G57" t="s">
-        <v>168</v>
-      </c>
-      <c r="H57" t="s">
-        <v>169</v>
-      </c>
-      <c r="I57" t="s">
-        <v>170</v>
-      </c>
-      <c r="J57" t="s">
-        <v>173</v>
-      </c>
-      <c r="K57" t="s">
-        <v>174</v>
-      </c>
-      <c r="O57" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>178</v>
-      </c>
-      <c r="V57" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.2">
@@ -6457,36 +6489,77 @@
         <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
         <v>47</v>
       </c>
       <c r="E58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" t="s">
+        <v>167</v>
+      </c>
+      <c r="G58" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58" t="s">
+        <v>169</v>
+      </c>
+      <c r="I58" t="s">
+        <v>170</v>
+      </c>
+      <c r="J58" t="s">
+        <v>173</v>
+      </c>
+      <c r="K58" t="s">
+        <v>174</v>
+      </c>
+      <c r="O58" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>178</v>
+      </c>
+      <c r="V58" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" t="s">
         <v>172</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>166</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>169</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H59" t="s">
         <v>170</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I59" t="s">
         <v>173</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J59" t="s">
         <v>174</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O59" t="s">
         <v>179</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="Q59" t="s">
         <v>177</v>
       </c>
-      <c r="V58" t="s">
+      <c r="V59" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
binding motifs report based on amino-acid strings command with alignment columns selector. Also, small update to the relevant binding locations for antibody HCV1
</commit_message>
<xml_diff>
--- a/tabular/antibodyEpitopeTable.xlsx
+++ b/tabular/antibodyEpitopeTable.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="246">
   <si>
     <t xml:space="preserve">Epitope </t>
   </si>
@@ -5189,7 +5189,7 @@
   <dimension ref="B1:V59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:O4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5368,6 +5368,12 @@
       <c r="E7" t="s">
         <v>4</v>
       </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
       <c r="H7" t="s">
         <v>7</v>
       </c>

</xml_diff>